<commit_message>
Faculty data base formatted
</commit_message>
<xml_diff>
--- a/CSE_faculty_formatted.xlsx
+++ b/CSE_faculty_formatted.xlsx
@@ -49,13 +49,13 @@
     <t xml:space="preserve">Mr.D.Ashok Reddy</t>
   </si>
   <si>
-    <t xml:space="preserve">CSE-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE-3</t>
+    <t xml:space="preserve">CSE-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSE-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSE-03</t>
   </si>
   <si>
     <t xml:space="preserve">23EC2109</t>
@@ -64,13 +64,13 @@
     <t xml:space="preserve">Mr. N. Mohan Rao</t>
   </si>
   <si>
-    <t xml:space="preserve">CSE-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE-6</t>
+    <t xml:space="preserve">CSE-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSE-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSE-06</t>
   </si>
   <si>
     <t xml:space="preserve">DLD</t>
@@ -556,8 +556,8 @@
   </sheetPr>
   <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P144" activeCellId="0" sqref="P144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>